<commit_message>
change print language from English to Japanese
</commit_message>
<xml_diff>
--- a/Reculcuration sheet.xlsx
+++ b/Reculcuration sheet.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="11320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -614,7 +612,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,7 +697,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,6 +720,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -781,7 +785,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -816,7 +820,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -993,7 +997,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1003,13 +1007,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1022,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>200000</v>
+        <v>10000</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>64</v>
@@ -1064,7 +1068,7 @@
       </c>
       <c r="B6">
         <f>B2/B3/B5</f>
-        <v>88.731144631765744</v>
+        <v>4.4365572315882869</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1084,7 +1088,7 @@
       </c>
       <c r="B8">
         <f>B6*(B4/(B4+1))</f>
-        <v>54.603781311855847</v>
+        <v>2.7301890655927918</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1093,7 +1097,7 @@
       </c>
       <c r="B9">
         <f>B8/B7</f>
-        <v>4.789805378232969E-2</v>
+        <v>2.3949026891164839E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1113,7 +1117,7 @@
       </c>
       <c r="B11">
         <f>B6*(1/(B4+1))</f>
-        <v>34.127363319909897</v>
+        <v>1.7063681659954948</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1122,7 +1126,7 @@
       </c>
       <c r="B12">
         <f>B11/B10</f>
-        <v>4.3253945906096193E-2</v>
+        <v>2.1626972953048096E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1152,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1161,7 +1165,7 @@
       </c>
       <c r="B18">
         <f>B17/B7/B5*10^6</f>
-        <v>268.5284640171858</v>
+        <v>143.21518080916576</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1170,7 +1174,7 @@
       </c>
       <c r="B19">
         <f>B20*60</f>
-        <v>2.4</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1178,7 +1182,7 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>0.04</v>
+        <v>2.0999999999999999E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1186,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>300</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1200,7 +1204,7 @@
       </c>
       <c r="B25">
         <f>B15*B19^0.5/B18^0.75</f>
-        <v>700.62257991884837</v>
+        <v>257.22592376309603</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1209,7 +1213,7 @@
       </c>
       <c r="B26">
         <f>B16*B20^0.5/(B5*B18)^0.75</f>
-        <v>1.7100844811312668</v>
+        <v>0.62783882932073842</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1226,8 +1230,8 @@
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="2">
-        <v>0.1</v>
+      <c r="B30" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1236,7 +1240,7 @@
       </c>
       <c r="B31">
         <f>B30/B10/B5*10^6</f>
-        <v>12.932929825922766</v>
+        <v>129.32929825922764</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1273,7 +1277,7 @@
       </c>
       <c r="B35">
         <f>B31-B34-B33-B32</f>
-        <v>8.8853625100230218</v>
+        <v>125.2817309433279</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1338,7 +1342,7 @@
       </c>
       <c r="B44">
         <f>(1/60)^2*(4*PI())^(2/3)/2/B5*(B15*SQRT(B19)/(1-B42^2)^0.5*B40)*(B38+B39+B38/B40^2)</f>
-        <v>5.0662590581538876</v>
+        <v>1.1608257812122933</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1356,7 +1360,7 @@
       </c>
       <c r="B46">
         <f>B15^(2/3)*B19^(1/3)/B45/B43^(2/3)</f>
-        <v>54.865918015273415</v>
+        <v>20.544192921198775</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1365,7 +1369,7 @@
       </c>
       <c r="B47">
         <f>1.1/SQRT(1-B42^2)*(B19/B15)^(1/3)</f>
-        <v>5.4729991722620559E-2</v>
+        <v>2.0493296188211538E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1374,7 +1378,7 @@
       </c>
       <c r="B48">
         <f>B47*B42</f>
-        <v>2.736499586131028E-2</v>
+        <v>1.0246648094105769E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1451,16 +1455,16 @@
       </c>
       <c r="B60">
         <f>B25*B59/2320</f>
-        <v>0.96637597230185979</v>
+        <v>0.35479437760427041</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B61">
-        <f>B56*B62^3-0.5*B62-B60^2*_xlfn.COT(RADIANS(B53))</f>
-        <v>-1.9413121412791783</v>
+      <c r="B61" t="e">
+        <f ca="1">B56*B62^3-0.5*B62-B60^2*_xlfn.COT(RADIANS(B53))</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1487,36 +1491,36 @@
       <c r="A64" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B64">
-        <f>(B56*B62-B63)/_xlfn.COT(RADIANS(B53))</f>
-        <v>3.9502351824923704E-2</v>
+      <c r="B64" t="e">
+        <f ca="1">(B56*B62-B63)/_xlfn.COT(RADIANS(B53))</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B65">
-        <f>SQRT(B64^2+B63^2)</f>
-        <v>0.58860266355989421</v>
+      <c r="B65" t="e">
+        <f ca="1">SQRT(B64^2+B63^2)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B66">
-        <f>B64/SIN(RADIANS(B53))</f>
-        <v>9.3470527426381456E-2</v>
+      <c r="B66" t="e">
+        <f ca="1">B64/SIN(RADIANS(B53))</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B67">
-        <f>DEGREES(ATAN(B64/B63))</f>
-        <v>3.8481315884567233</v>
+      <c r="B67" t="e">
+        <f ca="1">DEGREES(ATAN(B64/B63))</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1527,6 +1531,11 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>